<commit_message>
working programs: dc_appt_log and test_dc_appt_log
</commit_message>
<xml_diff>
--- a/dc.xlsx
+++ b/dc.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-18630" yWindow="6110" windowWidth="17820" windowHeight="13630" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -434,22 +433,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>6003</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>7034</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>98765432</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>7035</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>12345678</t>
+          <t>98745632</t>
         </is>
       </c>
     </row>

</xml_diff>